<commit_message>
change order of items
</commit_message>
<xml_diff>
--- a/storage/app/categories.xlsx
+++ b/storage/app/categories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cankert/Entwicklung/ShoppingApp/storage/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1A4D77-5FF8-F540-9A3E-EBA124C8F6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E163430C-ADC5-3D4C-94CB-187E4D1BD6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18940" yWindow="2940" windowWidth="25600" windowHeight="14180" xr2:uid="{0232B3AA-4449-734B-A677-8E458C88EE32}"/>
   </bookViews>
@@ -448,7 +448,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -581,7 +581,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -589,7 +589,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>